<commit_message>
stellar parameters and values.py
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="1"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="16700" windowHeight="9600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="transit-times" sheetId="1" r:id="rId1"/>
     <sheet name="ephem-sinukoff16" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="stellar-sme" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>i_planet</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Spitzer</t>
   </si>
   <si>
-    <t>Livingston reduction</t>
-  </si>
-  <si>
     <t>per1</t>
   </si>
   <si>
@@ -170,6 +168,51 @@
   </si>
   <si>
     <t>dur3_err</t>
+  </si>
+  <si>
+    <t>Livingston reduction; email 2/26; adopted larger of the asymetric uncerts</t>
+  </si>
+  <si>
+    <t>steff</t>
+  </si>
+  <si>
+    <t>steff_err</t>
+  </si>
+  <si>
+    <t>slogg</t>
+  </si>
+  <si>
+    <t>slogg_err</t>
+  </si>
+  <si>
+    <t>smet</t>
+  </si>
+  <si>
+    <t>smet_err</t>
+  </si>
+  <si>
+    <t>smass</t>
+  </si>
+  <si>
+    <t>smass_err</t>
+  </si>
+  <si>
+    <t>srad</t>
+  </si>
+  <si>
+    <t>srad_err</t>
+  </si>
+  <si>
+    <t>Brewer+16</t>
+  </si>
+  <si>
+    <t>srho</t>
+  </si>
+  <si>
+    <t>srho_err</t>
+  </si>
+  <si>
+    <t>Brewer+16 + isoclassify</t>
   </si>
 </sst>
 </file>
@@ -179,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +253,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -283,12 +332,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -627,14 +684,14 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -653,7 +710,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -962,7 +1019,7 @@
       <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -982,7 +1039,7 @@
       <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1002,7 +1059,7 @@
       <c r="E21" t="s">
         <v>9</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1022,7 +1079,7 @@
       <c r="E22" t="s">
         <v>10</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1042,11 +1099,11 @@
       <c r="E23" t="s">
         <v>12</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1057,13 +1114,13 @@
         <v>2457866.860415</v>
       </c>
       <c r="D24" s="2">
-        <v>8.4500000000000005E-4</v>
+        <v>8.8999999999999995E-4</v>
       </c>
       <c r="E24" t="s">
         <v>22</v>
       </c>
-      <c r="F24" t="s">
-        <v>23</v>
+      <c r="F24" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1079,7 +1136,7 @@
       <c r="D25" s="2">
         <v>4.6699166763600003E-2</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1096,11 +1153,11 @@
       <c r="D26" s="2">
         <v>0.15812975913300001</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1111,13 +1168,13 @@
         <v>2457852.477438</v>
       </c>
       <c r="D27" s="2">
-        <v>6.1510000000000002E-3</v>
+        <v>7.3509999999999999E-3</v>
       </c>
       <c r="E27" t="s">
         <v>22</v>
       </c>
-      <c r="F27" t="s">
-        <v>23</v>
+      <c r="F27" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1133,7 +1190,7 @@
       <c r="D28" s="2">
         <v>6.6393166314799995E-2</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1150,7 +1207,7 @@
       <c r="D29" s="2">
         <v>6.7601883318299999E-2</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1167,7 +1224,7 @@
       <c r="D30" s="2">
         <v>0.23201340204099999</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1184,11 +1241,51 @@
       <c r="D31" s="2">
         <v>0.23885614844</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>150</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2458001.5368400002</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.3619999999999999E-3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>102</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2458030.864513</v>
+      </c>
+      <c r="D33" s="2">
+        <v>5.9020000000000001E-3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C39" s="2"/>
     </row>
   </sheetData>
@@ -1201,7 +1298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1212,10 +1309,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1223,18 +1320,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>7.9194000000000004</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>5.0000000000000002E-5</v>
@@ -1242,18 +1339,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>813.38369999999998</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>2.9999999999999997E-4</v>
@@ -1261,18 +1358,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>3.5019999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>6.3E-2</v>
@@ -1280,7 +1377,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>11.90715</v>
@@ -1288,7 +1385,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>1.5E-3</v>
@@ -1296,7 +1393,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>817.27549999999997</v>
@@ -1304,7 +1401,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>5.1000000000000004E-3</v>
@@ -1312,7 +1409,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>4.3710000000000004</v>
@@ -1320,7 +1417,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1328,7 +1425,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>2.5085600000000001</v>
@@ -1336,7 +1433,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>4.0999999999999999E-4</v>
@@ -1344,7 +1441,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>808.92070000000001</v>
@@ -1352,7 +1449,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>8.6E-3</v>
@@ -1360,7 +1457,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>2.17</v>
@@ -1368,7 +1465,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>0.32800000000000001</v>
@@ -1482,4 +1579,151 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1">
+        <v>5322</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6">
+        <v>4.51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>0.04</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>0.04</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>0.87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>0.03</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>0.86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>0.04</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>1.37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>0.18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added in code to make tables
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petigura/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petigura/Research/K2-19_TTV+RV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="1040" windowWidth="22500" windowHeight="16760"/>
+    <workbookView xWindow="5440" yWindow="460" windowWidth="22500" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="transit-times" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>i_planet</t>
   </si>
@@ -204,6 +204,21 @@
   </si>
   <si>
     <t>Reduction by Nestor Espinoza, transit looks good</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>ref_key</t>
   </si>
 </sst>
 </file>
@@ -260,7 +275,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -281,6 +296,17 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -323,7 +349,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -340,6 +366,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -676,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -689,7 +718,7 @@
     <col min="6" max="6" width="36.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,8 +737,17 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -725,8 +763,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -745,8 +786,11 @@
       <c r="F3" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -762,8 +806,11 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -779,8 +826,11 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -796,8 +846,11 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -813,8 +866,11 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -830,8 +886,11 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -847,8 +906,11 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -864,8 +926,11 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -881,8 +946,11 @@
       <c r="E11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -898,8 +966,11 @@
       <c r="E12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -915,8 +986,11 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -932,8 +1006,11 @@
       <c r="E14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -949,8 +1026,11 @@
       <c r="E15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -966,8 +1046,11 @@
       <c r="E16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -983,8 +1066,11 @@
       <c r="E17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1000,8 +1086,11 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1020,8 +1109,14 @@
       <c r="F19" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1040,8 +1135,14 @@
       <c r="F20" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1060,8 +1161,14 @@
       <c r="F21" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1080,8 +1187,11 @@
       <c r="F22" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1100,8 +1210,14 @@
       <c r="F23" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1120,8 +1236,14 @@
       <c r="F24" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1140,8 +1262,14 @@
       <c r="F25" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>1</v>
       </c>
@@ -1160,8 +1288,14 @@
       <c r="F26" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="G26" s="7">
+        <v>1</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1180,8 +1314,14 @@
       <c r="F27" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1199,6 +1339,12 @@
       </c>
       <c r="F28" s="4" t="s">
         <v>36</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
keplerian fitting and nbody
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30040" yWindow="580" windowWidth="24540" windowHeight="19560"/>
+    <workbookView xWindow="10800" yWindow="460" windowWidth="24540" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="transit-times" sheetId="1" r:id="rId1"/>
@@ -193,9 +193,6 @@
     <t>Don't use. we missed the transit. Preliminary reduction by Leo Liu injected a transit in where there shouldn't have been one</t>
   </si>
   <si>
-    <t>Preliminary reduction Suvrath and Gummi, transit looks good</t>
-  </si>
-  <si>
     <t>Don't remember where these times came from, either a fit by Petigura or from some paper</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>Narita+15</t>
+  </si>
+  <si>
+    <t>APO observations by Suvrath and Gummi, intially it looks like they saw the transit, but further inspection revealed that there wasn't any detection</t>
   </si>
 </sst>
 </file>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -773,13 +773,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -819,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1142,13 +1142,13 @@
         <v>6</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1168,13 +1168,13 @@
         <v>7</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1194,13 +1194,13 @@
         <v>8</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -1226,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1243,13 +1243,13 @@
         <v>10</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1275,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1321,13 +1321,13 @@
         <v>51</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" s="7">
         <v>1</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
@@ -1403,7 +1403,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1">
         <v>4.2430000000000002E-3</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>1.1479999999999999E-3</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>33.984397999999999</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>4.6991139999999998</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>20.387806999999999</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>0.312</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>0.4859</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>6.3149999999999998E-2</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9">
         <v>6.7900000000000002E-4</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>2.6999999999999999E-5</v>
@@ -1534,7 +1534,7 @@
         <v>4.6699166763600003E-2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1551,7 +1551,7 @@
         <v>0.15812975913300001</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1568,7 +1568,7 @@
         <v>6.6393166314799995E-2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1585,7 +1585,7 @@
         <v>6.7601883318299999E-2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1602,7 +1602,7 @@
         <v>0.23201340204099999</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1619,7 +1619,7 @@
         <v>0.23885614844</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1974,7 +1974,7 @@
         <v>5322</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1985,7 +1985,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1996,7 +1996,7 @@
         <v>4.51</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2007,7 +2007,7 @@
         <v>0.08</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2018,7 +2018,7 @@
         <v>0.06</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2029,7 +2029,7 @@
         <v>0.05</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2040,7 +2040,7 @@
         <v>0.88</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2051,7 +2051,7 @@
         <v>0.03</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2062,7 +2062,7 @@
         <v>0.82</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2073,7 +2073,7 @@
         <v>0.04</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated with new livingston times
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="460" windowWidth="24540" windowHeight="17460"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="33780" windowHeight="20600"/>
   </bookViews>
   <sheets>
     <sheet name="transit-times" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>i_planet</t>
   </si>
@@ -142,9 +142,6 @@
     <t>dur3_err</t>
   </si>
   <si>
-    <t>Livingston reduction; email 2/26; adopted larger of the asymetric uncerts</t>
-  </si>
-  <si>
     <t>steff</t>
   </si>
   <si>
@@ -254,6 +251,12 @@
   </si>
   <si>
     <t>APO observations by Suvrath and Gummi, intially it looks like they saw the transit, but further inspection revealed that there wasn't any detection</t>
+  </si>
+  <si>
+    <t>Livingston reduction; email 11/7; adopted larger of the asymetric uncerts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -345,8 +348,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -406,7 +413,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -425,6 +432,8 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -443,6 +452,8 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,7 +754,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -773,13 +784,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -819,7 +830,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1142,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1168,13 +1179,13 @@
         <v>7</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1194,13 +1205,13 @@
         <v>8</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -1220,7 +1231,7 @@
         <v>9</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1243,13 +1254,13 @@
         <v>10</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1260,22 +1271,22 @@
         <v>133</v>
       </c>
       <c r="C24" s="2">
-        <v>2457866.860415</v>
+        <v>2457866.8607000001</v>
       </c>
       <c r="D24" s="2">
-        <v>8.8999999999999995E-4</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1286,22 +1297,22 @@
         <v>87</v>
       </c>
       <c r="C25" s="2">
-        <v>2457852.477438</v>
+        <v>2457852.4709999999</v>
       </c>
       <c r="D25" s="2">
-        <v>7.3509999999999999E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1318,16 +1329,16 @@
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" s="7">
         <v>1</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1338,22 +1349,22 @@
         <v>150</v>
       </c>
       <c r="C27" s="2">
-        <v>2458001.5368400002</v>
+        <v>2458001.5370999998</v>
       </c>
       <c r="D27" s="2">
-        <v>1.3619999999999999E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1364,25 +1375,30 @@
         <v>102</v>
       </c>
       <c r="C28" s="2">
-        <v>2458030.864513</v>
+        <v>2458030.8629999999</v>
       </c>
       <c r="D28" s="2">
-        <v>5.9020000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C39" s="2"/>
     </row>
   </sheetData>
@@ -1403,7 +1419,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1">
         <v>4.2430000000000002E-3</v>
@@ -1411,7 +1427,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>1.1479999999999999E-3</v>
@@ -1419,7 +1435,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>33.984397999999999</v>
@@ -1427,7 +1443,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>4.6991139999999998</v>
@@ -1435,7 +1451,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>20.387806999999999</v>
@@ -1443,7 +1459,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>0.312</v>
@@ -1451,7 +1467,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>0.4859</v>
@@ -1459,7 +1475,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>6.3149999999999998E-2</v>
@@ -1467,7 +1483,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>6.7900000000000002E-4</v>
@@ -1475,7 +1491,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>2.6999999999999999E-5</v>
@@ -1534,7 +1550,7 @@
         <v>4.6699166763600003E-2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1551,7 +1567,7 @@
         <v>0.15812975913300001</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1568,7 +1584,7 @@
         <v>6.6393166314799995E-2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1585,7 +1601,7 @@
         <v>6.7601883318299999E-2</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1602,7 +1618,7 @@
         <v>0.23201340204099999</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -1619,7 +1635,7 @@
         <v>0.23885614844</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1821,134 +1837,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1">
         <v>5322</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6">
         <v>4.51</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>0.05</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>0.04</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>0.87</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>0.03</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>0.86</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>0.04</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>1.37</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0.18</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1968,112 +1984,112 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1">
         <v>5322</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6">
         <v>4.51</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>0.08</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>0.06</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>0.05</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>0.88</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>0.03</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>0.82</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>0.04</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>